<commit_message>
Add prepare draw logic
</commit_message>
<xml_diff>
--- a/Product/SettingSource/food_card.xlsx
+++ b/Product/SettingSource/food_card.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -83,6 +83,10 @@
   </si>
   <si>
     <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOOD_DESC_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,7 +436,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -509,6 +513,9 @@
       </c>
       <c r="E4">
         <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suppot TexturePacker.Use UIAtlas to render immage from imageset.
</commit_message>
<xml_diff>
--- a/Product/SettingSource/food_card.xlsx
+++ b/Product/SettingSource/food_card.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>FOOD_DESC_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simple_atlas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simple_tex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩略图集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩略图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardSimple</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -433,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -444,7 +468,7 @@
     <col min="2" max="2" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +487,14 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -483,8 +513,14 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -503,8 +539,14 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -516,6 +558,9 @@
       </c>
       <c r="F4" t="s">
         <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>